<commit_message>
update readme and part comments.
</commit_message>
<xml_diff>
--- a/experiment/result/PG数据库实验.xlsx
+++ b/experiment/result/PG数据库实验.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\Rl-Study\controller\experiment\result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\ppo-controller\experiment\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BA7015-50F6-47A9-9EF5-D03548C3B9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95D814C-E9BF-4D50-A61E-DED83D841FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="353" windowWidth="19396" windowHeight="11745" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45972" yWindow="4488" windowWidth="30936" windowHeight="17496" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="4" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="sheet5" sheetId="8" r:id="rId6"/>
     <sheet name="sheet6" sheetId="9" r:id="rId7"/>
     <sheet name="sheet7" sheetId="10" r:id="rId8"/>
+    <sheet name="sheet3-1" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="38">
   <si>
     <t>Smopdc</t>
   </si>
@@ -170,6 +171,10 @@
   <si>
     <t>Optimal</t>
   </si>
+  <si>
+    <t>OPT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -272,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -314,12 +319,6 @@
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -336,6 +335,16 @@
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1759,13 +1768,13 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="2" width="10.59765625" customWidth="1"/>
-    <col min="5" max="5" width="20.265625" customWidth="1"/>
+    <col min="2" max="2" width="10.58203125" customWidth="1"/>
+    <col min="5" max="5" width="20.25" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1783,7 +1792,7 @@
         <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1997,13 +2006,13 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="5" max="5" width="15.265625" customWidth="1"/>
-    <col min="6" max="6" width="17.06640625" customWidth="1"/>
+    <col min="5" max="5" width="15.25" customWidth="1"/>
+    <col min="6" max="6" width="17.08203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2020,7 +2029,7 @@
         <v>17</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2241,14 +2250,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CD31AD-4505-422E-850A-90340DE93486}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30:Q36"/>
+    <sheetView topLeftCell="D17" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="3" max="3" width="12.1328125" customWidth="1"/>
-    <col min="7" max="7" width="18.1328125" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2507,41 +2516,41 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:20">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18" t="s">
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26" t="s">
         <v>29</v>
       </c>
       <c r="J19" s="5"/>
-      <c r="M19" s="17" t="s">
+      <c r="M19" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="N19" s="17"/>
-      <c r="O19" s="18" t="s">
+      <c r="N19" s="27"/>
+      <c r="O19" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18" t="s">
+      <c r="P19" s="26"/>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="26"/>
+      <c r="T19" s="26" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:20">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="1" t="s">
         <v>2</v>
       </c>
@@ -2557,11 +2566,11 @@
       <c r="H20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="18"/>
+      <c r="I20" s="26"/>
       <c r="J20" s="5"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
       <c r="O20" s="1" t="s">
         <v>2</v>
       </c>
@@ -2577,20 +2586,20 @@
       <c r="S20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T20" s="18"/>
+      <c r="T20" s="26"/>
     </row>
     <row r="21" spans="1:20">
       <c r="C21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
       <c r="M21" s="5" t="s">
         <v>20</v>
       </c>
@@ -2598,33 +2607,33 @@
         <f t="shared" ref="N21:S21" si="1">SUM(C22:C24)</f>
         <v>520</v>
       </c>
-      <c r="O21" s="19">
+      <c r="O21" s="17">
         <f t="shared" si="1"/>
         <v>205.74801199999999</v>
       </c>
-      <c r="P21" s="19">
+      <c r="P21" s="17">
         <f t="shared" si="1"/>
         <v>132.69379599999999</v>
       </c>
-      <c r="Q21" s="19">
+      <c r="Q21" s="17">
         <f t="shared" si="1"/>
         <v>146.54722610000002</v>
       </c>
-      <c r="R21" s="20">
+      <c r="R21" s="18">
         <f t="shared" si="1"/>
         <v>131.04211500000002</v>
       </c>
-      <c r="S21" s="19">
+      <c r="S21" s="17">
         <f t="shared" si="1"/>
         <v>189.41717199999999</v>
       </c>
-      <c r="T21" s="19">
+      <c r="T21" s="17">
         <f>AVERAGE(O21:S21)</f>
         <v>161.08966421999997</v>
       </c>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="26" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2659,33 +2668,33 @@
         <f t="shared" ref="N22:S22" si="2">SUM(C25:C27)</f>
         <v>1200</v>
       </c>
-      <c r="O22" s="19">
+      <c r="O22" s="17">
         <f t="shared" si="2"/>
         <v>38.018540000000002</v>
       </c>
-      <c r="P22" s="19">
+      <c r="P22" s="17">
         <f t="shared" si="2"/>
         <v>38.485552000000006</v>
       </c>
-      <c r="Q22" s="20">
+      <c r="Q22" s="18">
         <f t="shared" si="2"/>
         <v>29.562405999999999</v>
       </c>
-      <c r="R22" s="19">
+      <c r="R22" s="17">
         <f t="shared" si="2"/>
         <v>72.530787000000004</v>
       </c>
-      <c r="S22" s="19">
+      <c r="S22" s="17">
         <f t="shared" si="2"/>
         <v>40.222931199999998</v>
       </c>
-      <c r="T22" s="19">
+      <c r="T22" s="17">
         <f t="shared" ref="T22:T23" si="3">AVERAGE(O22:S22)</f>
         <v>43.764043239999999</v>
       </c>
     </row>
     <row r="23" spans="1:20">
-      <c r="A23" s="18"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
@@ -2718,33 +2727,33 @@
         <f t="shared" ref="N23:S23" si="5">SUM(C28:C31)</f>
         <v>1680</v>
       </c>
-      <c r="O23" s="19">
+      <c r="O23" s="17">
         <f t="shared" si="5"/>
         <v>92.742834999999999</v>
       </c>
-      <c r="P23" s="19">
+      <c r="P23" s="17">
         <f t="shared" si="5"/>
         <v>68.030349999999999</v>
       </c>
-      <c r="Q23" s="20">
+      <c r="Q23" s="18">
         <f t="shared" si="5"/>
         <v>53.613504999999989</v>
       </c>
-      <c r="R23" s="19">
+      <c r="R23" s="17">
         <f t="shared" si="5"/>
         <v>142.30719999999999</v>
       </c>
-      <c r="S23" s="19">
+      <c r="S23" s="17">
         <f t="shared" si="5"/>
         <v>67.830160000000006</v>
       </c>
-      <c r="T23" s="19">
+      <c r="T23" s="17">
         <f t="shared" si="3"/>
         <v>84.904809999999998</v>
       </c>
     </row>
     <row r="24" spans="1:20">
-      <c r="A24" s="18"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
@@ -2777,30 +2786,30 @@
         <f>AVERAGE(N21:N23)</f>
         <v>1133.3333333333333</v>
       </c>
-      <c r="O24" s="19">
+      <c r="O24" s="17">
         <f t="shared" ref="O24:S24" si="6">AVERAGE(O21:O23)</f>
         <v>112.16979566666667</v>
       </c>
-      <c r="P24" s="19">
+      <c r="P24" s="17">
         <f t="shared" si="6"/>
         <v>79.736565999999996</v>
       </c>
-      <c r="Q24" s="20">
+      <c r="Q24" s="18">
         <f t="shared" si="6"/>
         <v>76.574379033333344</v>
       </c>
-      <c r="R24" s="19">
+      <c r="R24" s="17">
         <f t="shared" si="6"/>
         <v>115.29336733333334</v>
       </c>
-      <c r="S24" s="19">
+      <c r="S24" s="17">
         <f t="shared" si="6"/>
         <v>99.156754399999997</v>
       </c>
-      <c r="T24" s="19"/>
+      <c r="T24" s="17"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="26" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2830,7 +2839,7 @@
       </c>
     </row>
     <row r="26" spans="1:20">
-      <c r="A26" s="18"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
@@ -2859,7 +2868,7 @@
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:20">
-      <c r="A27" s="18"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
@@ -2888,7 +2897,7 @@
       <c r="M27" s="5"/>
     </row>
     <row r="28" spans="1:20">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="26" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2918,7 +2927,7 @@
       </c>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="18"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="1" t="s">
         <v>10</v>
       </c>
@@ -2944,10 +2953,10 @@
         <f t="shared" si="4"/>
         <v>43.913902</v>
       </c>
-      <c r="M29" s="22"/>
+      <c r="M29" s="20"/>
     </row>
     <row r="30" spans="1:20">
-      <c r="A30" s="18"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="1" t="s">
         <v>11</v>
       </c>
@@ -2973,22 +2982,22 @@
         <f t="shared" si="4"/>
         <v>23.026520000000001</v>
       </c>
-      <c r="M30" s="22"/>
-      <c r="N30" s="21" t="s">
+      <c r="M30" s="20"/>
+      <c r="N30" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="O30" s="21" t="s">
+      <c r="O30" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="P30" s="21" t="s">
+      <c r="P30" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="Q30" s="21" t="s">
+      <c r="Q30" s="19" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:20">
-      <c r="A31" s="18"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="1" t="s">
         <v>12</v>
       </c>
@@ -3014,27 +3023,27 @@
         <f t="shared" si="4"/>
         <v>17.793084</v>
       </c>
-      <c r="M31" s="21" t="s">
+      <c r="M31" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="N31" s="23">
+      <c r="N31" s="21">
         <v>205.74799999999999</v>
       </c>
-      <c r="O31" s="23">
+      <c r="O31" s="21">
         <v>38.018540000000002</v>
       </c>
-      <c r="P31" s="23">
+      <c r="P31" s="21">
         <v>92.742840000000001</v>
       </c>
-      <c r="Q31" s="23">
+      <c r="Q31" s="21">
         <v>112.1698</v>
       </c>
     </row>
     <row r="32" spans="1:20">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="18"/>
+      <c r="B32" s="26"/>
       <c r="C32">
         <f>AVERAGEA(C22:C31)</f>
         <v>340</v>
@@ -3059,125 +3068,125 @@
         <f t="shared" si="7"/>
         <v>29.747026319999996</v>
       </c>
-      <c r="M32" s="21" t="s">
+      <c r="M32" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="N32" s="23">
+      <c r="N32" s="21">
         <v>132.69380000000001</v>
       </c>
-      <c r="O32" s="23">
+      <c r="O32" s="21">
         <v>38.485550000000003</v>
       </c>
-      <c r="P32" s="23">
+      <c r="P32" s="21">
         <v>68.030349999999999</v>
       </c>
-      <c r="Q32" s="23">
+      <c r="Q32" s="21">
         <v>79.73657</v>
       </c>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
-      <c r="M33" s="21" t="s">
+      <c r="M33" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="N33" s="23">
+      <c r="N33" s="21">
         <v>146.5472</v>
       </c>
-      <c r="O33" s="24">
+      <c r="O33" s="22">
         <v>29.56241</v>
       </c>
-      <c r="P33" s="24">
+      <c r="P33" s="22">
         <v>53.613509999999998</v>
       </c>
-      <c r="Q33" s="24">
+      <c r="Q33" s="22">
         <v>76.574380000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="25.5">
-      <c r="M34" s="21" t="s">
+    <row r="34" spans="1:17" ht="26">
+      <c r="M34" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="N34" s="24">
+      <c r="N34" s="22">
         <v>131.0421</v>
       </c>
-      <c r="O34" s="23">
+      <c r="O34" s="21">
         <v>72.530789999999996</v>
       </c>
-      <c r="P34" s="23">
+      <c r="P34" s="21">
         <v>142.30719999999999</v>
       </c>
-      <c r="Q34" s="23">
+      <c r="Q34" s="21">
         <v>115.29340000000001</v>
       </c>
     </row>
     <row r="35" spans="1:17">
-      <c r="M35" s="21" t="s">
+      <c r="M35" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="N35" s="23">
+      <c r="N35" s="21">
         <v>189.41720000000001</v>
       </c>
-      <c r="O35" s="23">
+      <c r="O35" s="21">
         <v>40.222929999999998</v>
       </c>
-      <c r="P35" s="23">
+      <c r="P35" s="21">
         <v>67.830160000000006</v>
       </c>
-      <c r="Q35" s="23">
+      <c r="Q35" s="21">
         <v>99.156750000000002</v>
       </c>
     </row>
     <row r="36" spans="1:17">
-      <c r="M36" s="21" t="s">
+      <c r="M36" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="N36" s="23">
+      <c r="N36" s="21">
         <v>161.08969999999999</v>
       </c>
-      <c r="O36" s="23">
+      <c r="O36" s="21">
         <v>43.764040000000001</v>
       </c>
-      <c r="P36" s="23">
+      <c r="P36" s="21">
         <v>84.904809999999998</v>
       </c>
-      <c r="Q36" s="25"/>
+      <c r="Q36" s="23"/>
     </row>
     <row r="37" spans="1:17" ht="13.9" customHeight="1"/>
     <row r="38" spans="1:17">
-      <c r="M38" s="21"/>
-      <c r="N38" s="24"/>
-      <c r="O38" s="23"/>
-      <c r="P38" s="23"/>
-      <c r="Q38" s="23"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="21"/>
     </row>
     <row r="40" spans="1:17">
-      <c r="M40" s="21"/>
-      <c r="N40" s="23"/>
-      <c r="O40" s="23"/>
-      <c r="P40" s="23"/>
-      <c r="Q40" s="23"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="21"/>
     </row>
     <row r="42" spans="1:17">
-      <c r="M42" s="21"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="23"/>
-      <c r="Q42" s="25"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="21"/>
+      <c r="Q42" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="M19:N20"/>
     <mergeCell ref="T19:T20"/>
     <mergeCell ref="O19:S19"/>
     <mergeCell ref="D21:H21"/>
     <mergeCell ref="A19:C20"/>
     <mergeCell ref="D19:H19"/>
     <mergeCell ref="I19:I21"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="M19:N20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3192,9 +3201,9 @@
       <selection activeCell="D2" sqref="D2:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="16.1328125" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
   </cols>
@@ -3466,9 +3475,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3672,10 +3681,10 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" customWidth="1"/>
-    <col min="2" max="2" width="15.06640625" customWidth="1"/>
+    <col min="1" max="1" width="12.58203125" customWidth="1"/>
+    <col min="2" max="2" width="15.08203125" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3944,13 +3953,13 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="22.1328125" customWidth="1"/>
-    <col min="2" max="2" width="16.73046875" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" customWidth="1"/>
-    <col min="4" max="4" width="18.9296875" customWidth="1"/>
-    <col min="5" max="5" width="24.73046875" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
+    <col min="3" max="3" width="15.58203125" customWidth="1"/>
+    <col min="4" max="4" width="18.9140625" customWidth="1"/>
+    <col min="5" max="5" width="24.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4230,7 +4239,7 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -4351,6 +4360,240 @@
       </c>
       <c r="C11">
         <v>379.58</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC5A43F-0494-44D3-9345-5D02C6ABD798}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="24">
+        <v>11.508012000000001</v>
+      </c>
+      <c r="C2" s="24">
+        <v>8.1691739999999999</v>
+      </c>
+      <c r="D2" s="24">
+        <v>7.3203581</v>
+      </c>
+      <c r="E2" s="25">
+        <v>1.165999</v>
+      </c>
+      <c r="F2" s="24">
+        <v>9.8011619999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="24">
+        <v>134.13999999999999</v>
+      </c>
+      <c r="C3" s="24">
+        <v>99.271000000000001</v>
+      </c>
+      <c r="D3" s="24">
+        <v>95.876286000000007</v>
+      </c>
+      <c r="E3" s="25">
+        <v>59.176116000000007</v>
+      </c>
+      <c r="F3" s="24">
+        <v>120.81908999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="24">
+        <v>60.1</v>
+      </c>
+      <c r="C4" s="24">
+        <v>25.253622</v>
+      </c>
+      <c r="D4" s="24">
+        <v>43.350581999999996</v>
+      </c>
+      <c r="E4" s="25">
+        <v>70.7</v>
+      </c>
+      <c r="F4" s="24">
+        <v>58.79692</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="24">
+        <v>22.701000000000001</v>
+      </c>
+      <c r="C5" s="24">
+        <v>21.99954</v>
+      </c>
+      <c r="D5" s="24">
+        <v>14.876060999999998</v>
+      </c>
+      <c r="E5" s="25">
+        <v>53.534637000000004</v>
+      </c>
+      <c r="F5" s="24">
+        <v>20.073119999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="15">
+        <v>14.746679999999998</v>
+      </c>
+      <c r="C6" s="15">
+        <v>16.20355</v>
+      </c>
+      <c r="D6" s="15">
+        <v>13.425360000000001</v>
+      </c>
+      <c r="E6" s="15">
+        <v>18.882249999999999</v>
+      </c>
+      <c r="F6" s="15">
+        <v>19.685549999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="15">
+        <v>0.57086000000000003</v>
+      </c>
+      <c r="C7" s="15">
+        <v>0.28246200000000005</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1.260985</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.1139</v>
+      </c>
+      <c r="F7" s="15">
+        <v>0.46426120000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15">
+        <v>0.15151500000000001</v>
+      </c>
+      <c r="C8" s="15">
+        <v>7.5050000000000006E-2</v>
+      </c>
+      <c r="D8" s="15">
+        <v>0.25955499999999998</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.16839999999999999</v>
+      </c>
+      <c r="F8" s="15">
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="15">
+        <v>53.134639999999997</v>
+      </c>
+      <c r="C9" s="15">
+        <v>41.173100000000005</v>
+      </c>
+      <c r="D9" s="15">
+        <v>32.485049999999994</v>
+      </c>
+      <c r="E9" s="24">
+        <v>54.000799999999998</v>
+      </c>
+      <c r="F9" s="15">
+        <v>38.775920000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="15">
+        <v>23.32668</v>
+      </c>
+      <c r="C10" s="15">
+        <v>14.706099999999999</v>
+      </c>
+      <c r="D10" s="15">
+        <v>11.688299999999998</v>
+      </c>
+      <c r="E10" s="24">
+        <v>50.31</v>
+      </c>
+      <c r="F10" s="15">
+        <v>15.101520000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="15">
+        <v>16.13</v>
+      </c>
+      <c r="C11" s="15">
+        <v>12.0761</v>
+      </c>
+      <c r="D11" s="15">
+        <v>9.1806000000000001</v>
+      </c>
+      <c r="E11" s="15">
+        <v>37.828000000000003</v>
+      </c>
+      <c r="F11" s="15">
+        <v>13.750719999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>